<commit_message>
update productiedossier en timesheet
</commit_message>
<xml_diff>
--- a/docs/timesheet_Tine_Vancoillie.xlsx
+++ b/docs/timesheet_Tine_Vancoillie.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13640" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17600" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Datum</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>Wireflow</t>
+  </si>
+  <si>
+    <t>Analyse + dossier</t>
+  </si>
+  <si>
+    <t>Aanpassingen dossier</t>
+  </si>
+  <si>
+    <t>Analyse</t>
   </si>
 </sst>
 </file>
@@ -176,7 +185,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -197,6 +206,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent5" xfId="3" builtinId="45"/>
@@ -477,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -529,7 +539,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="21" thickTop="1" thickBot="1">
@@ -540,7 +550,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="10">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21" thickTop="1" thickBot="1">
@@ -562,7 +572,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="10">
-        <v>5.25</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21" thickTop="1" thickBot="1">
@@ -595,7 +605,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="10">
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21" thickTop="1" thickBot="1">
@@ -606,58 +616,86 @@
         <v>15</v>
       </c>
       <c r="C11" s="10">
-        <v>4.75</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21" thickTop="1" thickBot="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="7">
+        <v>42660</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="21" thickTop="1" thickBot="1">
-      <c r="A13" s="7">
-        <v>42660</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2"/>
+      <c r="A13" s="9">
+        <v>42390</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="10">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="21" thickTop="1" thickBot="1">
-      <c r="A14" s="7">
+      <c r="A14" s="9">
+        <v>42665</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="10">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="12" customFormat="1" ht="21" thickTop="1" thickBot="1">
+      <c r="A15" s="9">
+        <v>42666</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="10">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="21" thickTop="1" thickBot="1">
+      <c r="A16" s="7">
         <v>42709</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" ht="21" thickTop="1" thickBot="1">
-      <c r="A15" s="7">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="21" thickTop="1" thickBot="1">
+      <c r="A17" s="7">
         <v>42731</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" ht="17" thickTop="1" thickBot="1">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5" t="s">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" ht="17" thickTop="1" thickBot="1">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="3">
-        <f>SUM(C3:C15)</f>
+      <c r="C18" s="3">
+        <f>SUM(C3:C17)</f>
         <v>32.5</v>
       </c>
     </row>
-    <row r="17" ht="16" thickTop="1"/>
-    <row r="35" ht="46" customHeight="1"/>
-    <row r="36" ht="17" customHeight="1"/>
-    <row r="37" ht="17" customHeight="1"/>
+    <row r="19" spans="1:3" ht="16" thickTop="1"/>
+    <row r="37" ht="46" customHeight="1"/>
     <row r="38" ht="17" customHeight="1"/>
     <row r="39" ht="17" customHeight="1"/>
     <row r="40" ht="17" customHeight="1"/>
+    <row r="41" ht="17" customHeight="1"/>
+    <row r="42" ht="17" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>

</xml_diff>